<commit_message>
Front polish 20 mins
</commit_message>
<xml_diff>
--- a/Tabela za vodjenja taskova za test projekat (Autosaved).xlsx
+++ b/Tabela za vodjenja taskova za test projekat (Autosaved).xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="56">
   <si>
     <t>Naziv user storija</t>
   </si>
@@ -91,12 +91,6 @@
     <t>is blocked</t>
   </si>
   <si>
-    <t>balance</t>
-  </si>
-  <si>
-    <t>transaction type</t>
-  </si>
-  <si>
     <t>Kao korisnik potrebno je da mogu da vidim listu svojih transakcija</t>
   </si>
   <si>
@@ -208,6 +202,9 @@
   </si>
   <si>
     <t>webclient init &amp; config</t>
+  </si>
+  <si>
+    <t>5m</t>
   </si>
 </sst>
 </file>
@@ -547,8 +544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -576,7 +573,7 @@
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -584,22 +581,22 @@
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>5</v>
@@ -610,7 +607,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>5</v>
@@ -621,7 +618,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>5</v>
@@ -632,13 +629,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -665,13 +662,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -687,35 +684,35 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D14" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C15" t="s">
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s">
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -731,21 +728,30 @@
       <c r="C18" t="s">
         <v>5</v>
       </c>
+      <c r="D18" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
+      </c>
+      <c r="D19" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C20" t="s">
         <v>5</v>
+      </c>
+      <c r="D20" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -755,32 +761,35 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C22" t="s">
         <v>9</v>
+      </c>
+      <c r="D22" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C23" t="s">
         <v>9</v>
+      </c>
+      <c r="D23" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E24" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C25" t="s">
         <v>9</v>
@@ -788,7 +797,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C26" t="s">
         <v>15</v>
@@ -796,23 +805,20 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C27" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E28" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C29" t="s">
         <v>9</v>
@@ -823,10 +829,13 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C30" t="s">
-        <v>44</v>
+        <v>42</v>
+      </c>
+      <c r="D30" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -840,15 +849,15 @@
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C32" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C33" t="s">
         <v>9</v>
@@ -856,7 +865,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C34" t="s">
         <v>9</v>
@@ -864,12 +873,12 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C36" t="s">
         <v>9</v>
@@ -877,7 +886,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C37" t="s">
         <v>5</v>
@@ -885,12 +894,12 @@
     </row>
     <row r="38" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C39" t="s">
         <v>15</v>
@@ -898,23 +907,23 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C40" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E41" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C42" t="s">
         <v>11</v>
@@ -922,81 +931,81 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C43" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C44" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C46" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C47" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C48" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C50" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C51" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C52" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C53" t="s">
         <v>11</v>
@@ -1004,7 +1013,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C54" t="s">
         <v>5</v>
@@ -1012,15 +1021,15 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C56" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
@@ -1031,7 +1040,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C59" t="s">
         <v>5</v>
@@ -1039,7 +1048,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Webclient moved to correct folder
</commit_message>
<xml_diff>
--- a/Tabela za vodjenja taskova za test projekat (Autosaved).xlsx
+++ b/Tabela za vodjenja taskova za test projekat (Autosaved).xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="61">
   <si>
     <t>Naziv user storija</t>
   </si>
@@ -100,9 +100,6 @@
     <t>Administrator moze da blokira/odblokira odredjeni novcanik/nalog</t>
   </si>
   <si>
-    <t>uvodjenje rola I admina</t>
-  </si>
-  <si>
     <t>20m</t>
   </si>
   <si>
@@ -208,6 +205,21 @@
   </si>
   <si>
     <t>/</t>
+  </si>
+  <si>
+    <t>implementacija usecasea</t>
+  </si>
+  <si>
+    <t>dodavanje config-a za admina</t>
+  </si>
+  <si>
+    <t>konfiguracija webclienta</t>
+  </si>
+  <si>
+    <t>0m</t>
+  </si>
+  <si>
+    <t>25m</t>
   </si>
 </sst>
 </file>
@@ -547,8 +559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -576,7 +588,7 @@
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -584,22 +596,22 @@
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>5</v>
@@ -610,7 +622,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>5</v>
@@ -621,7 +633,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>5</v>
@@ -632,13 +644,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -665,13 +677,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" t="s">
         <v>38</v>
       </c>
-      <c r="C12" t="s">
-        <v>39</v>
-      </c>
       <c r="D12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -687,10 +699,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>
@@ -698,24 +710,24 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C16" t="s">
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -737,7 +749,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
@@ -748,13 +760,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C20" t="s">
         <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -764,24 +776,24 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C22" t="s">
         <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C23" t="s">
         <v>9</v>
       </c>
       <c r="D23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -792,18 +804,18 @@
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C25" t="s">
         <v>9</v>
       </c>
       <c r="D25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C26" t="s">
         <v>15</v>
@@ -814,13 +826,13 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -830,7 +842,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C29" t="s">
         <v>9</v>
@@ -841,13 +853,13 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -861,26 +873,35 @@
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32" t="s">
         <v>43</v>
       </c>
-      <c r="C32" t="s">
-        <v>44</v>
+      <c r="D32" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C33" t="s">
         <v>9</v>
+      </c>
+      <c r="D33" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C34" t="s">
         <v>9</v>
+      </c>
+      <c r="D34" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -890,18 +911,24 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C36" t="s">
         <v>9</v>
+      </c>
+      <c r="D36" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C37" t="s">
         <v>5</v>
+      </c>
+      <c r="D37" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -911,7 +938,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C39" t="s">
         <v>15</v>
@@ -919,10 +946,10 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C40" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
@@ -930,35 +957,41 @@
         <v>20</v>
       </c>
       <c r="E41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="C42" t="s">
-        <v>11</v>
+        <v>43</v>
+      </c>
+      <c r="D42" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="C43" t="s">
-        <v>22</v>
+        <v>41</v>
+      </c>
+      <c r="D43" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B44" t="s">
-        <v>46</v>
-      </c>
-      <c r="C44" t="s">
+      <c r="A44" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
+      <c r="B45" t="s">
+        <v>44</v>
+      </c>
+      <c r="C45" t="s">
         <v>24</v>
       </c>
     </row>
@@ -967,28 +1000,28 @@
         <v>45</v>
       </c>
       <c r="C46" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="C47" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B48" t="s">
-        <v>27</v>
-      </c>
-      <c r="C48" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A49" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A48" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
+        <v>44</v>
+      </c>
+      <c r="C49" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
@@ -996,71 +1029,71 @@
         <v>45</v>
       </c>
       <c r="C50" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="C51" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B52" t="s">
-        <v>27</v>
+      <c r="A52" t="s">
+        <v>47</v>
       </c>
       <c r="C52" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
+        <v>36</v>
+      </c>
+      <c r="C53" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C55" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C53" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>37</v>
-      </c>
-      <c r="C54" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>50</v>
-      </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C56" s="1" t="s">
-        <v>49</v>
-      </c>
+      <c r="C56" s="1"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C57" s="1"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C58" s="1"/>
+      <c r="A58" t="s">
+        <v>50</v>
+      </c>
+      <c r="C58" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>51</v>
       </c>
-      <c r="C59" t="s">
-        <v>5</v>
+      <c r="C59" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Renamed methods in transaction
</commit_message>
<xml_diff>
--- a/Tabela za vodjenja taskova za test projekat (Autosaved).xlsx
+++ b/Tabela za vodjenja taskova za test projekat (Autosaved).xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="59">
   <si>
     <t>Naziv user storija</t>
   </si>
@@ -88,9 +88,6 @@
 </t>
   </si>
   <si>
-    <t>is blocked</t>
-  </si>
-  <si>
     <t>Kao korisnik potrebno je da mogu da vidim listu svojih transakcija</t>
   </si>
   <si>
@@ -175,9 +172,6 @@
   </si>
   <si>
     <t>usecase impl (front-end)</t>
-  </si>
-  <si>
-    <t>admin rola?</t>
   </si>
   <si>
     <t>testovi</t>
@@ -557,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E60"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -588,7 +582,7 @@
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -596,22 +590,22 @@
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>34</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>5</v>
@@ -622,7 +616,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>5</v>
@@ -633,7 +627,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>5</v>
@@ -644,13 +638,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -677,13 +671,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" t="s">
         <v>37</v>
       </c>
-      <c r="C12" t="s">
-        <v>38</v>
-      </c>
       <c r="D12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -699,10 +693,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>
@@ -710,32 +704,32 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C15" t="s">
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C16" t="s">
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" t="s">
         <v>14</v>
@@ -747,75 +741,75 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
         <v>44</v>
       </c>
-      <c r="C19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
-        <v>45</v>
-      </c>
       <c r="C20" t="s">
         <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
         <v>44</v>
       </c>
-      <c r="C22" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
-        <v>45</v>
-      </c>
       <c r="C23" t="s">
         <v>9</v>
       </c>
       <c r="D23" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C25" t="s">
         <v>9</v>
       </c>
       <c r="D25" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C26" t="s">
         <v>15</v>
@@ -824,278 +818,272 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D27" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
         <v>44</v>
       </c>
-      <c r="C29" t="s">
-        <v>9</v>
-      </c>
-      <c r="D29" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B30" t="s">
-        <v>45</v>
-      </c>
       <c r="C30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D30" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E31" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" t="s">
         <v>42</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
         <v>43</v>
       </c>
-      <c r="D32" t="s">
+      <c r="C33" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B33" t="s">
+      <c r="C36" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
         <v>44</v>
       </c>
-      <c r="C33" t="s">
-        <v>9</v>
-      </c>
-      <c r="D33" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B34" t="s">
-        <v>45</v>
-      </c>
-      <c r="C34" t="s">
-        <v>9</v>
-      </c>
-      <c r="D34" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+      <c r="C37" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B36" t="s">
-        <v>44</v>
-      </c>
-      <c r="C36" t="s">
-        <v>9</v>
-      </c>
-      <c r="D36" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B37" t="s">
-        <v>45</v>
-      </c>
-      <c r="C37" t="s">
-        <v>5</v>
-      </c>
-      <c r="D37" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="15" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B39" t="s">
-        <v>44</v>
       </c>
       <c r="C39" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C40" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>55</v>
+      </c>
+      <c r="C42" t="s">
+        <v>42</v>
+      </c>
+      <c r="D42" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>54</v>
+      </c>
+      <c r="C43" t="s">
+        <v>40</v>
+      </c>
+      <c r="D43" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>43</v>
+      </c>
+      <c r="C45" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
+        <v>44</v>
+      </c>
+      <c r="C46" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>20</v>
-      </c>
-      <c r="E41" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B42" t="s">
-        <v>57</v>
-      </c>
-      <c r="C42" t="s">
-        <v>43</v>
-      </c>
-      <c r="D42" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B43" t="s">
-        <v>56</v>
-      </c>
-      <c r="C43" t="s">
-        <v>41</v>
-      </c>
-      <c r="D43" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B45" t="s">
-        <v>44</v>
-      </c>
-      <c r="C45" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>25</v>
+      </c>
+      <c r="C47" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A48" s="3" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B46" t="s">
-        <v>45</v>
-      </c>
-      <c r="C46" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B47" t="s">
-        <v>26</v>
-      </c>
-      <c r="C47" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A48" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C49" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C50" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C51" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>47</v>
+      <c r="A52" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="C52" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>36</v>
+      <c r="A53" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="C53" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="C55" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C56" s="1"/>
+      <c r="C56" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C57" s="1"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>50</v>
-      </c>
-      <c r="C58" t="s">
-        <v>5</v>
-      </c>
+      <c r="C58" s="1"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>51</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>9</v>
+        <v>48</v>
+      </c>
+      <c r="C59" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C60" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>56</v>
+      </c>
+      <c r="C61" s="4" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed typo in webclient namming Webbclient to Webclient
</commit_message>
<xml_diff>
--- a/Tabela za vodjenja taskova za test projekat (Autosaved).xlsx
+++ b/Tabela za vodjenja taskova za test projekat (Autosaved).xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="73">
   <si>
     <t>Naziv user storija</t>
   </si>
@@ -114,9 +114,6 @@
     <t>estimacija taskova</t>
   </si>
   <si>
-    <t>postavljanje foldera projekata</t>
-  </si>
-  <si>
     <t>2h</t>
   </si>
   <si>
@@ -126,18 +123,6 @@
     <t>crtanje I razmisljanje</t>
   </si>
   <si>
-    <t>ukupno</t>
-  </si>
-  <si>
-    <t>ef core edukacija</t>
-  </si>
-  <si>
-    <t>4h</t>
-  </si>
-  <si>
-    <t>docker edukacija</t>
-  </si>
-  <si>
     <t>dokerizacija</t>
   </si>
   <si>
@@ -147,9 +132,6 @@
     <t>15 min</t>
   </si>
   <si>
-    <t>provera da li je punoletan</t>
-  </si>
-  <si>
     <t>uvodjenje transfera</t>
   </si>
   <si>
@@ -165,12 +147,6 @@
     <t>testovi</t>
   </si>
   <si>
-    <t xml:space="preserve"> samo code                  1330</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> sa pred pocetkom    1630</t>
-  </si>
-  <si>
     <t>configuracija baze</t>
   </si>
   <si>
@@ -180,9 +156,6 @@
     <t>65m</t>
   </si>
   <si>
-    <t>webclient init &amp; config</t>
-  </si>
-  <si>
     <t>5m</t>
   </si>
   <si>
@@ -207,9 +180,6 @@
     <t>vizualizacija</t>
   </si>
   <si>
-    <t>usecase impl</t>
-  </si>
-  <si>
     <t>usecase implementacija</t>
   </si>
   <si>
@@ -223,6 +193,69 @@
   </si>
   <si>
     <t>configuracija</t>
+  </si>
+  <si>
+    <t>postavljanje foldera projekta</t>
+  </si>
+  <si>
+    <t>jmbg check</t>
+  </si>
+  <si>
+    <t>80m</t>
+  </si>
+  <si>
+    <t>195m</t>
+  </si>
+  <si>
+    <t>1110m</t>
+  </si>
+  <si>
+    <t>1425m</t>
+  </si>
+  <si>
+    <t>estimacija razmisljanje crtanje</t>
+  </si>
+  <si>
+    <t>samo zadatak</t>
+  </si>
+  <si>
+    <t>1330m</t>
+  </si>
+  <si>
+    <t>1630m</t>
+  </si>
+  <si>
+    <t>usecase implementacija provera stanja na novcaniku</t>
+  </si>
+  <si>
+    <t>usecase implementacija - uvesti check svuda osim pregleda transakcija I pregleda novcanika</t>
+  </si>
+  <si>
+    <t>usecase implementacija - izlistati transakcije</t>
+  </si>
+  <si>
+    <t>usecase implementacija - promena pass-a</t>
+  </si>
+  <si>
+    <t>usecase implementacija - withdraw money</t>
+  </si>
+  <si>
+    <t>usecase impl - deposit money</t>
+  </si>
+  <si>
+    <t>usecase implementacija - transfer money</t>
+  </si>
+  <si>
+    <t>implementacija usecasea - uvodjenje pravila</t>
+  </si>
+  <si>
+    <t>docker edukacija (nije uzeto u obzir)</t>
+  </si>
+  <si>
+    <t>ef core edukacija (nije uzeto u obzir)</t>
+  </si>
+  <si>
+    <t>webclient init &amp; config (I trazenje templatea)</t>
   </si>
 </sst>
 </file>
@@ -560,17 +593,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D62"/>
+  <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="67.6640625" customWidth="1"/>
-    <col min="2" max="2" width="35.33203125" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="2" max="2" width="36.88671875" customWidth="1"/>
+    <col min="3" max="3" width="39.44140625" customWidth="1"/>
     <col min="4" max="4" width="22.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -591,26 +624,26 @@
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>31</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="C3" s="4"/>
       <c r="D3" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" s="1"/>
     </row>
@@ -627,7 +660,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>5</v>
@@ -638,7 +671,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>5</v>
@@ -649,13 +682,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
-        <v>47</v>
+        <v>72</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -682,13 +715,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" t="s">
         <v>34</v>
-      </c>
-      <c r="C12" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -704,18 +737,18 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="C14" t="s">
         <v>20</v>
       </c>
       <c r="D14" t="s">
-        <v>5</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="C15" t="s">
         <v>9</v>
@@ -726,13 +759,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s">
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -754,7 +787,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
@@ -765,7 +798,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C20" t="s">
         <v>5</v>
@@ -781,24 +814,24 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="C22" t="s">
         <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C23" t="s">
         <v>9</v>
       </c>
       <c r="D23" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -809,18 +842,18 @@
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C25" t="s">
         <v>9</v>
       </c>
       <c r="D25" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="C26" t="s">
         <v>15</v>
@@ -831,13 +864,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C27" t="s">
         <v>21</v>
       </c>
       <c r="D27" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -847,7 +880,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C29" t="s">
         <v>9</v>
@@ -858,10 +891,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C30" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D30" t="s">
         <v>20</v>
@@ -875,35 +908,35 @@
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C32" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D32" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C33" t="s">
         <v>9</v>
       </c>
       <c r="D33" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C34" t="s">
         <v>9</v>
       </c>
       <c r="D34" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -913,24 +946,24 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="C36" t="s">
         <v>9</v>
       </c>
       <c r="D36" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C37" t="s">
         <v>5</v>
       </c>
       <c r="D37" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15" x14ac:dyDescent="0.3">
@@ -940,7 +973,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="C39" t="s">
         <v>15</v>
@@ -951,13 +984,13 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C40" t="s">
         <v>20</v>
       </c>
       <c r="D40" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -967,21 +1000,21 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C42" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D42" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C43" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D43" t="s">
         <v>9</v>
@@ -994,7 +1027,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="C45" t="s">
         <v>5</v>
@@ -1005,24 +1038,24 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C46" t="s">
         <v>21</v>
       </c>
       <c r="D46" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C47" t="s">
         <v>21</v>
       </c>
       <c r="D47" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -1032,7 +1065,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="C49" t="s">
         <v>5</v>
@@ -1043,106 +1076,128 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C50" t="s">
         <v>21</v>
       </c>
       <c r="D50" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C51" t="s">
         <v>21</v>
       </c>
       <c r="D51" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C52" t="s">
         <v>11</v>
       </c>
+      <c r="D52" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C53" t="s">
         <v>5</v>
       </c>
+      <c r="D53" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>43</v>
-      </c>
+      <c r="C55" s="1"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C56" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="A56" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C56" s="1"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C57" s="1"/>
+      <c r="A57" t="s">
+        <v>36</v>
+      </c>
+      <c r="C57" t="s">
+        <v>5</v>
+      </c>
+      <c r="D57" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C58" s="1"/>
+      <c r="A58" t="s">
+        <v>37</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D58" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>44</v>
-      </c>
-      <c r="C59" t="s">
+        <v>48</v>
+      </c>
+      <c r="C59" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D59" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D60" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
+      <c r="C61" s="4"/>
+      <c r="D61" s="1"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" s="1"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C61" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D61" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>59</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D62" t="s">
-        <v>9</v>
+      <c r="C65" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>